<commit_message>
updated blueprint spreadsheet accdg to new site instructions
</commit_message>
<xml_diff>
--- a/design/service blueprint source files/NSF-SBIR-blueprint-current/NSF-SBIR-service-blueprint-current.xlsx
+++ b/design/service blueprint source files/NSF-SBIR-blueprint-current/NSF-SBIR-service-blueprint-current.xlsx
@@ -7,15 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Current state (March 2017)" sheetId="1" r:id="rId4"/>
+    <sheet name="Current state (March 2017)-1" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="140">
-  <si>
-    <t>Table 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="155">
   <si>
     <t>Phase</t>
   </si>
@@ -77,19 +75,34 @@
     <t>Sign up for newsletter (listserv)</t>
   </si>
   <si>
+    <t>Determine if company is a good fit.</t>
+  </si>
+  <si>
+    <t>Read technology topic areas</t>
+  </si>
+  <si>
     <t>Research and figure out other awardees</t>
   </si>
   <si>
-    <t>Watch videos</t>
-  </si>
-  <si>
-    <t>Read technology topic areas</t>
-  </si>
-  <si>
-    <t>Submit Executive Summary</t>
-  </si>
-  <si>
-    <t>Read solicitation.</t>
+    <t>Watch videos (i.e., archived webinars)</t>
+  </si>
+  <si>
+    <t>Register firm with NSF Fastlane (requires EIN, DUNS)</t>
+  </si>
+  <si>
+    <t>Read current solicitation.</t>
+  </si>
+  <si>
+    <t>Read FastLane submission guide.</t>
+  </si>
+  <si>
+    <t>Read funding criteria.</t>
+  </si>
+  <si>
+    <t>Click on link to view Phase I awards</t>
+  </si>
+  <si>
+    <t>Solicit pre-submission feedback (Executive Summary)</t>
   </si>
   <si>
     <t>Attend webinar.</t>
@@ -147,15 +160,12 @@
     </r>
   </si>
   <si>
-    <t>Register firm with NSF Fastlane (requires EIN, DUNS)</t>
+    <t>Enter information into FastLane</t>
   </si>
   <si>
     <t>Begin to gather letters of support.</t>
   </si>
   <si>
-    <t>Enter information into FastLane</t>
-  </si>
-  <si>
     <t>PI and Administrator certification</t>
   </si>
   <si>
@@ -165,9 +175,6 @@
     <t>Submit proposal</t>
   </si>
   <si>
-    <t>Waiting</t>
-  </si>
-  <si>
     <t>Respond to email(s).</t>
   </si>
   <si>
@@ -195,9 +202,6 @@
     <t>Customer able to access remaining funding</t>
   </si>
   <si>
-    <t>Apply for Phase II</t>
-  </si>
-  <si>
     <t>Touchpoints &amp; Devices</t>
   </si>
   <si>
@@ -348,7 +352,88 @@
     <t>NSF SBIR website</t>
   </si>
   <si>
-    <t xml:space="preserve">NSF SBIR awards search </t>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>NSF SBIR good fit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="9"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.nsf.gov/eng/iip/sbir/goodfit.jsp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>NSF SBIR topics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="9"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.nsf.gov/eng/iip/sbir/topics.jsp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>NSF SBIR Portfolio</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="9"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.nsf.gov/eng/iip/sbir/portfolio.jsp</t>
+    </r>
   </si>
   <si>
     <t>Reaching out to network to see if they know NSF SBIR</t>
@@ -363,7 +448,163 @@
     <t>LinkedIn</t>
   </si>
   <si>
-    <t>NSF SBIR website / YouTube</t>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">NSF SBIR website / YouTube: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="9"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.nsf.gov/eng/iip/sbir/Webinar/PhaseI.jsp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Online</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.fastlane.nsf.gov/a0/about/registration.htm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>NSF SBIR recent call</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="9"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.nsf.gov/eng/iip/sbir/recent_call.jsp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>NSF SBIR website</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="9"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.nsf.gov/eng/iip/sbir/fastlane1.jsp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>NSF SBIR website</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="9"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.nsf.gov/eng/iip/sbir/peer_review.jsp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>NSF SBIR website</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="9"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.nsf.gov/awardsearch/advancedSearchResult?ProgEleCode=5371%2C1505&amp;BooleanElement=Any&amp;ActiveAwards=true</t>
+    </r>
   </si>
   <si>
     <t>Emails (PD contact info obtained from website)</t>
@@ -486,38 +727,10 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="9"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>Online</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="9"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>https://www.fastlane.nsf.gov/a0/about/registration.htm</t>
-    </r>
+    <t>FastLane</t>
   </si>
   <si>
     <t>??</t>
-  </si>
-  <si>
-    <t>FastLane</t>
   </si>
   <si>
     <t>Phone</t>
@@ -726,7 +939,7 @@
 </t>
   </si>
   <si>
-    <t>How would your target audience learn about NSF SBIR at this stage? Solely through ads?</t>
+    <t>How does the target audience learn about NSF SBIR at this stage? Solely through ads?</t>
   </si>
   <si>
     <t xml:space="preserve">(1) There are no events or other time-based content on the site. (Even the submission deadlines tend to be buried.) (2) No system for managing contacts 
@@ -740,64 +953,171 @@
     <t>Users did not find the search listings or the available data on the companies very helpful.</t>
   </si>
   <si>
+    <t xml:space="preserve">(1) Takes 1-2 days turnaround. (2) Need to identify Principal Investigator (PI) </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Each solicitation only active ~60 days each year. Link points here: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="9"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.nsf.gov/eng/iip/sbir/recent_call.jsp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> which points to archived solicitation: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="9"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.nsf.gov/pubs/2016/nsf16599/nsf16599.htm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> which points to referee page:  </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="9"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.nsf.gov/publications/pub_summ.jsp?ods_key=nsf17544</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> which has a tiny link to the html view of the solicitation: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="9"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.nsf.gov/pubs/2017/nsf17544/nsf17544.htm</t>
+    </r>
+  </si>
+  <si>
     <t>Some email different PDs and get different answers from each. 10-12% of executive summaries fall through the cracks and are left unanswered. (This is sensitive; a known problem)</t>
   </si>
   <si>
+    <t>NSF SBIR is not allowed to conduct these until the solicitation has been posted. Registration captures email.</t>
+  </si>
+  <si>
+    <t>FAQs need to undergo legal review. Often updated shortly after each new solicitation is published.</t>
+  </si>
+  <si>
+    <t>(1) Takes 30 days for a free DUNS number or 5 days for a $50 fee.</t>
+  </si>
+  <si>
+    <t>(1) How long does this process take if you’re starting from scratch?</t>
+  </si>
+  <si>
+    <t>(1) May take 2-6 weeks turnaround.</t>
+  </si>
+  <si>
+    <t>Info includes: Outline of proposal (structured); Financials / Budget (structured); Refer to  Department of Labor/Bureau of Labor Statistics for salary ranges; Project Summary (structured); Personnel (structured); Resumes / CVs (unstructured); Cover Sheet (structured); Letters of Support (unstructured); Business Model (unstructured); Commercialization history / SBA Certification form (unstructured)</t>
+  </si>
+  <si>
+    <t>(1) Is there a template or a set of guidelines for this? (2) How is this currently submitted? (3) Can they submit soft copies? (4) Do the letters need to be notarized? I.e., how do you verify/authenticate?</t>
+  </si>
+  <si>
+    <t>(This is a known pain point as the applicant has to create another account to submit as a research administrator. Applications wind up being disqualified because they are deemed incomplete.)</t>
+  </si>
+  <si>
+    <t>(1) Help Desk receives hundreds of calls during peak period</t>
+  </si>
+  <si>
+    <t>Usually takes about 1 week. Reasons for RWR: (1) Projects which were submitted late (2) Projects with project descriptions &gt; 15 pages (if the extra pages have no significant content, we will usually let them go to panel, but if it looks like it’s too much to have put on 15 pages, they will be returned) (3) Projects asking for significantly more than $225,000 (4) Some projects which are completely missing a commercial discussion will get flagged by the staff and returned.</t>
+  </si>
+  <si>
+    <t>Decisions are final. No protests — but are allowed to submit another Phase I proposal. (1) Do applicants receive additional feedback on why they were rejected?</t>
+  </si>
+  <si>
+    <t>20% of the money is withheld until the very end of the Phase I period upon receipt of the final report.</t>
+  </si>
+  <si>
+    <t>Customer Value</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>–</t>
+  </si>
+  <si>
+    <t>NSF Value</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">NSF SBIR website: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="9"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.nsf.gov/eng/iip/sbir/topics.jsp</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">NSF SBIR awards search </t>
+  </si>
+  <si>
+    <t>Submit Executive Summary</t>
+  </si>
+  <si>
+    <t>Read current solicitation (if available).</t>
+  </si>
+  <si>
     <t>Each solicitation only active ~60 days each year.</t>
   </si>
   <si>
-    <t>NSF SBIR is not allowed to conduct these until the solicitation has been posted. Registration captures email.</t>
-  </si>
-  <si>
-    <t>FAQs need to undergo legal review</t>
-  </si>
-  <si>
-    <t>(1) Takes 30 days for a free DUNS number or 5 days for a $50 fee.</t>
-  </si>
-  <si>
-    <t>(1) How long does this process take if you’re starting from scratch?</t>
-  </si>
-  <si>
-    <t>(1) May take 2-6 weeks turnaround.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1) Takes 1-2 days turnaround. (2) Need to identify Principal Investigator (PI) </t>
-  </si>
-  <si>
-    <t>(1) Is there a template or a set of guidelines for this? (2) How is this currently submitted? (3) Can they submit soft copies? (4) Do the letters need to be notarized? I.e., how do you verify/authenticate?</t>
-  </si>
-  <si>
-    <t>Info includes: Outline of proposal (structured); Financials / Budget (structured); Refer to  Department of Labor/Bureau of Labor Statistics for salary ranges; Project Summary (structured); Personnel (structured); Resumes / CVs (unstructured); Cover Sheet (structured); Letters of Support (unstructured); Business Model (unstructured); Commercialization history / SBA Certification form (unstructured)</t>
-  </si>
-  <si>
-    <t>(This is a known pain point as the applicant has to create another account to submit as a research administrator. Applications wind up being disqualified because they are deemed incomplete.)</t>
-  </si>
-  <si>
-    <t>(1) Help Desk receives hundreds of calls during peak period</t>
-  </si>
-  <si>
-    <t>Usually takes about 1 week. Reasons for RWR: (1) Projects which were submitted late (2) Projects with project descriptions &gt; 15 pages (if the extra pages have no significant content, we will usually let them go to panel, but if it looks like it’s too much to have put on 15 pages, they will be returned) (3) Projects asking for significantly more than $225,000 (4) Some projects which are completely missing a commercial discussion will get flagged by the staff and returned.</t>
-  </si>
-  <si>
-    <t>Decisions are final. No protests — but are allowed to submit another Phase I proposal. (1) Do applicants receive additional feedback on why they were rejected?</t>
-  </si>
-  <si>
-    <t>20% of the money is withheld until the very end of the Phase I period upon receipt of the final report.</t>
-  </si>
-  <si>
-    <t>Customer Value</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>–</t>
-  </si>
-  <si>
-    <t>NSF Value</t>
+    <t>Attend webinar (if available).</t>
+  </si>
+  <si>
+    <t>Email from Kelly</t>
   </si>
 </sst>
 </file>
@@ -807,7 +1127,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -815,6 +1135,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
@@ -839,6 +1164,12 @@
       <u val="single"/>
       <sz val="9"/>
       <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="9"/>
+      <color indexed="15"/>
       <name val="Helvetica"/>
     </font>
     <font>
@@ -869,7 +1200,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="11"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -880,7 +1211,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -892,9 +1223,7 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
-      <right>
-        <color indexed="8"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="10"/>
       </top>
@@ -904,9 +1233,7 @@
       <diagonal/>
     </border>
     <border>
-      <left>
-        <color indexed="8"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -914,7 +1241,7 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -929,17 +1256,15 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left>
-        <color indexed="8"/>
+      <left style="thin">
+        <color indexed="14"/>
       </left>
-      <right>
-        <color indexed="8"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="10"/>
       </top>
@@ -949,14 +1274,12 @@
       <diagonal/>
     </border>
     <border>
-      <left>
-        <color indexed="8"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -971,7 +1294,7 @@
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -979,9 +1302,7 @@
       <diagonal/>
     </border>
     <border>
-      <left>
-        <color indexed="8"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -1008,69 +1329,258 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1089,11 +1599,13 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1110,10 +1622,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="404040"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="BFBFBF"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="499BC9"/>
@@ -1307,14 +1819,15 @@
   <a:objectDefaults>
     <a:spDef>
       <a:spPr>
-        <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
-          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
-        </a:blipFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst>
           <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
@@ -1329,7 +1842,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1344,20 +1857,14 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
-            <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
-                <a:srgbClr val="000000">
-                  <a:alpha val="31034"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
             <a:uFillTx/>
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
@@ -1610,14 +2117,20 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="6350" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1906,7 +2419,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -2187,11 +2700,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:BC16"/>
+  <dimension ref="A1:BF15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.6" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
@@ -2250,425 +2761,458 @@
     <col min="53" max="53" width="19.6016" style="1" customWidth="1"/>
     <col min="54" max="54" width="19.6016" style="1" customWidth="1"/>
     <col min="55" max="55" width="19.6016" style="1" customWidth="1"/>
-    <col min="56" max="256" width="19.6016" style="1" customWidth="1"/>
+    <col min="56" max="56" width="19.6016" style="1" customWidth="1"/>
+    <col min="57" max="57" width="19.6016" style="1" customWidth="1"/>
+    <col min="58" max="58" width="19.6016" style="1" customWidth="1"/>
+    <col min="59" max="256" width="19.6016" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28" customHeight="1">
+    <row r="1" ht="19.55" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="2"/>
-      <c r="AM1" s="2"/>
-      <c r="AN1" s="2"/>
-      <c r="AO1" s="2"/>
-      <c r="AP1" s="2"/>
-      <c r="AQ1" s="2"/>
-      <c r="AR1" s="2"/>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="2"/>
-      <c r="AU1" s="2"/>
-      <c r="AV1" s="2"/>
-      <c r="AW1" s="2"/>
-      <c r="AX1" s="2"/>
-      <c r="AY1" s="2"/>
-      <c r="AZ1" s="2"/>
-      <c r="BA1" s="2"/>
-      <c r="BB1" s="2"/>
-      <c r="BC1" s="2"/>
-    </row>
-    <row r="2" ht="19.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" t="s" s="6">
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" t="s" s="6">
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" t="s" s="6">
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6"/>
+      <c r="AM1" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5"/>
-      <c r="AI2" t="s" s="6">
+      <c r="AN1" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="AJ2" t="s" s="6">
+      <c r="AO1" t="s" s="5">
         <v>7</v>
       </c>
-      <c r="AK2" t="s" s="6">
+      <c r="AP1" s="4"/>
+      <c r="AQ1" s="4"/>
+      <c r="AR1" t="s" s="5">
         <v>8</v>
       </c>
-      <c r="AL2" s="5"/>
-      <c r="AM2" s="5"/>
-      <c r="AN2" t="s" s="6">
+      <c r="AS1" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="AO2" t="s" s="6">
+      <c r="AT1" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="AP2" t="s" s="6">
+      <c r="AU1" s="4"/>
+      <c r="AV1" t="s" s="5">
         <v>11</v>
       </c>
-      <c r="AQ2" s="5"/>
-      <c r="AR2" t="s" s="6">
+      <c r="AW1" s="7"/>
+      <c r="AX1" s="7"/>
+      <c r="AY1" s="7"/>
+      <c r="AZ1" s="7"/>
+      <c r="BA1" s="7"/>
+      <c r="BB1" s="7"/>
+      <c r="BC1" s="7"/>
+      <c r="BD1" s="7"/>
+      <c r="BE1" s="7"/>
+      <c r="BF1" s="7"/>
+    </row>
+    <row r="2" ht="63.55" customHeight="1">
+      <c r="A2" t="s" s="8">
         <v>12</v>
       </c>
-      <c r="AS2" s="7"/>
-      <c r="AT2" s="7"/>
-      <c r="AU2" s="7"/>
-      <c r="AV2" s="7"/>
-      <c r="AW2" s="7"/>
-      <c r="AX2" s="7"/>
-      <c r="AY2" s="7"/>
-      <c r="AZ2" s="7"/>
-      <c r="BA2" s="7"/>
-      <c r="BB2" s="7"/>
-      <c r="BC2" s="7"/>
-    </row>
-    <row r="3" ht="63.55" customHeight="1">
+      <c r="B2" t="s" s="9">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s" s="10">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s" s="10">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s" s="10">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s" s="11">
+        <v>17</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="13"/>
+      <c r="L2" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="M2" s="12"/>
+      <c r="N2" t="s" s="10">
+        <v>19</v>
+      </c>
+      <c r="O2" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="P2" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s" s="10">
+        <v>22</v>
+      </c>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" t="s" s="10">
+        <v>23</v>
+      </c>
+      <c r="W2" t="s" s="10">
+        <v>24</v>
+      </c>
+      <c r="X2" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="Y2" t="s" s="10">
+        <v>26</v>
+      </c>
+      <c r="Z2" t="s" s="10">
+        <v>27</v>
+      </c>
+      <c r="AA2" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="AB2" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="AC2" s="12"/>
+      <c r="AD2" t="s" s="10">
+        <v>30</v>
+      </c>
+      <c r="AE2" t="s" s="10">
+        <v>31</v>
+      </c>
+      <c r="AF2" t="s" s="10">
+        <v>32</v>
+      </c>
+      <c r="AG2" t="s" s="10">
+        <v>33</v>
+      </c>
+      <c r="AH2" t="s" s="10">
+        <v>34</v>
+      </c>
+      <c r="AI2" t="s" s="10">
+        <v>35</v>
+      </c>
+      <c r="AJ2" t="s" s="10">
+        <v>36</v>
+      </c>
+      <c r="AK2" t="s" s="10">
+        <v>37</v>
+      </c>
+      <c r="AL2" t="s" s="10">
+        <v>38</v>
+      </c>
+      <c r="AM2" t="s" s="10">
+        <v>39</v>
+      </c>
+      <c r="AN2" s="13"/>
+      <c r="AO2" s="10"/>
+      <c r="AP2" s="10"/>
+      <c r="AQ2" s="10"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" t="s" s="10">
+        <v>40</v>
+      </c>
+      <c r="AT2" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="AU2" s="10"/>
+      <c r="AV2" t="s" s="10">
+        <v>42</v>
+      </c>
+      <c r="AW2" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="AX2" t="s" s="10">
+        <v>44</v>
+      </c>
+      <c r="AY2" t="s" s="10">
+        <v>45</v>
+      </c>
+      <c r="AZ2" s="13"/>
+      <c r="BA2" s="13"/>
+      <c r="BB2" s="13"/>
+      <c r="BC2" s="13"/>
+      <c r="BD2" t="s" s="10">
+        <v>46</v>
+      </c>
+      <c r="BE2" t="s" s="10">
+        <v>47</v>
+      </c>
+      <c r="BF2" t="s" s="10">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" ht="96.35" customHeight="1">
       <c r="A3" t="s" s="8">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s" s="10">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="13"/>
-      <c r="L3" t="s" s="10">
-        <v>19</v>
-      </c>
-      <c r="M3" s="12"/>
-      <c r="N3" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="O3" t="s" s="10">
-        <v>21</v>
-      </c>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" t="s" s="10">
-        <v>22</v>
-      </c>
-      <c r="U3" t="s" s="10">
-        <v>23</v>
-      </c>
-      <c r="V3" t="s" s="10">
-        <v>24</v>
-      </c>
-      <c r="W3" s="12"/>
-      <c r="X3" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="Y3" t="s" s="10">
-        <v>26</v>
-      </c>
-      <c r="Z3" t="s" s="10">
-        <v>27</v>
-      </c>
-      <c r="AA3" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="AB3" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="AC3" t="s" s="10">
-        <v>30</v>
-      </c>
-      <c r="AD3" t="s" s="10">
-        <v>31</v>
-      </c>
-      <c r="AE3" t="s" s="10">
-        <v>32</v>
-      </c>
-      <c r="AF3" t="s" s="10">
-        <v>33</v>
-      </c>
-      <c r="AG3" t="s" s="10">
-        <v>34</v>
-      </c>
-      <c r="AH3" t="s" s="10">
-        <v>35</v>
-      </c>
-      <c r="AI3" t="s" s="10">
-        <v>36</v>
-      </c>
-      <c r="AJ3" s="13"/>
-      <c r="AK3" t="s" s="10">
-        <v>37</v>
-      </c>
-      <c r="AL3" t="s" s="10">
-        <v>37</v>
-      </c>
-      <c r="AM3" t="s" s="10">
-        <v>37</v>
-      </c>
-      <c r="AN3" t="s" s="10">
-        <v>37</v>
-      </c>
-      <c r="AO3" t="s" s="10">
-        <v>38</v>
-      </c>
-      <c r="AP3" t="s" s="10">
-        <v>39</v>
-      </c>
-      <c r="AQ3" t="s" s="10">
-        <v>37</v>
-      </c>
-      <c r="AR3" t="s" s="10">
-        <v>40</v>
-      </c>
-      <c r="AS3" t="s" s="10">
-        <v>41</v>
-      </c>
-      <c r="AT3" t="s" s="10">
-        <v>42</v>
-      </c>
-      <c r="AU3" t="s" s="10">
-        <v>43</v>
-      </c>
-      <c r="AV3" s="13"/>
-      <c r="AW3" s="13"/>
-      <c r="AX3" s="13"/>
-      <c r="AY3" s="13"/>
-      <c r="AZ3" t="s" s="10">
-        <v>44</v>
-      </c>
-      <c r="BA3" t="s" s="10">
-        <v>45</v>
-      </c>
-      <c r="BB3" t="s" s="10">
-        <v>46</v>
-      </c>
-      <c r="BC3" t="s" s="10">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" ht="96.35" customHeight="1">
+        <v>49</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" t="s" s="15">
+        <v>50</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" t="s" s="15">
+        <v>51</v>
+      </c>
+      <c r="G3" t="s" s="15">
+        <v>52</v>
+      </c>
+      <c r="H3" t="s" s="15">
+        <v>53</v>
+      </c>
+      <c r="I3" t="s" s="15">
+        <v>54</v>
+      </c>
+      <c r="J3" t="s" s="15">
+        <v>55</v>
+      </c>
+      <c r="K3" s="16"/>
+      <c r="L3" t="s" s="15">
+        <v>56</v>
+      </c>
+      <c r="M3" t="s" s="15">
+        <v>57</v>
+      </c>
+      <c r="N3" t="s" s="15">
+        <v>57</v>
+      </c>
+      <c r="O3" t="s" s="15">
+        <v>58</v>
+      </c>
+      <c r="P3" t="s" s="15">
+        <v>59</v>
+      </c>
+      <c r="Q3" t="s" s="15">
+        <v>60</v>
+      </c>
+      <c r="R3" t="s" s="15">
+        <v>61</v>
+      </c>
+      <c r="S3" t="s" s="15">
+        <v>62</v>
+      </c>
+      <c r="T3" t="s" s="17">
+        <v>63</v>
+      </c>
+      <c r="U3" t="s" s="17">
+        <v>64</v>
+      </c>
+      <c r="V3" t="s" s="15">
+        <v>65</v>
+      </c>
+      <c r="W3" t="s" s="15">
+        <v>66</v>
+      </c>
+      <c r="X3" t="s" s="15">
+        <v>67</v>
+      </c>
+      <c r="Y3" t="s" s="15">
+        <v>68</v>
+      </c>
+      <c r="Z3" t="s" s="15">
+        <v>69</v>
+      </c>
+      <c r="AA3" t="s" s="15">
+        <v>70</v>
+      </c>
+      <c r="AB3" t="s" s="15">
+        <v>71</v>
+      </c>
+      <c r="AC3" t="s" s="15">
+        <v>72</v>
+      </c>
+      <c r="AD3" t="s" s="15">
+        <v>73</v>
+      </c>
+      <c r="AE3" t="s" s="15">
+        <v>74</v>
+      </c>
+      <c r="AF3" t="s" s="15">
+        <v>75</v>
+      </c>
+      <c r="AG3" t="s" s="15">
+        <v>76</v>
+      </c>
+      <c r="AH3" t="s" s="15">
+        <v>77</v>
+      </c>
+      <c r="AI3" t="s" s="15">
+        <v>78</v>
+      </c>
+      <c r="AJ3" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="AK3" t="s" s="15">
+        <v>78</v>
+      </c>
+      <c r="AL3" t="s" s="15">
+        <v>80</v>
+      </c>
+      <c r="AM3" t="s" s="15">
+        <v>78</v>
+      </c>
+      <c r="AN3" s="16"/>
+      <c r="AO3" s="16"/>
+      <c r="AP3" s="16"/>
+      <c r="AQ3" s="16"/>
+      <c r="AR3" s="16"/>
+      <c r="AS3" t="s" s="15">
+        <v>81</v>
+      </c>
+      <c r="AT3" t="s" s="15">
+        <v>81</v>
+      </c>
+      <c r="AU3" s="16"/>
+      <c r="AV3" t="s" s="15">
+        <v>81</v>
+      </c>
+      <c r="AW3" t="s" s="15">
+        <v>82</v>
+      </c>
+      <c r="AX3" s="16"/>
+      <c r="AY3" s="16"/>
+      <c r="AZ3" s="16"/>
+      <c r="BA3" s="16"/>
+      <c r="BB3" s="16"/>
+      <c r="BC3" s="16"/>
+      <c r="BD3" t="s" s="15">
+        <v>83</v>
+      </c>
+      <c r="BE3" t="s" s="15">
+        <v>84</v>
+      </c>
+      <c r="BF3" t="s" s="15">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" ht="74.35" customHeight="1">
       <c r="A4" t="s" s="8">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" t="s" s="15">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
-      <c r="F4" t="s" s="15">
-        <v>50</v>
-      </c>
-      <c r="G4" t="s" s="15">
-        <v>51</v>
-      </c>
-      <c r="H4" t="s" s="15">
-        <v>52</v>
-      </c>
-      <c r="I4" t="s" s="15">
-        <v>53</v>
-      </c>
-      <c r="J4" t="s" s="15">
-        <v>54</v>
-      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
       <c r="K4" s="16"/>
-      <c r="L4" t="s" s="15">
-        <v>55</v>
-      </c>
-      <c r="M4" t="s" s="15">
-        <v>56</v>
-      </c>
-      <c r="N4" t="s" s="15">
-        <v>56</v>
-      </c>
-      <c r="O4" t="s" s="15">
-        <v>57</v>
-      </c>
-      <c r="P4" t="s" s="15">
-        <v>58</v>
-      </c>
-      <c r="Q4" t="s" s="15">
-        <v>59</v>
-      </c>
-      <c r="R4" t="s" s="15">
-        <v>60</v>
-      </c>
-      <c r="S4" t="s" s="15">
-        <v>61</v>
-      </c>
-      <c r="T4" t="s" s="15">
-        <v>62</v>
-      </c>
-      <c r="U4" t="s" s="15">
-        <v>56</v>
-      </c>
-      <c r="V4" t="s" s="15">
-        <v>63</v>
-      </c>
-      <c r="W4" t="s" s="15">
-        <v>64</v>
-      </c>
-      <c r="X4" t="s" s="15">
-        <v>56</v>
-      </c>
-      <c r="Y4" t="s" s="15">
-        <v>65</v>
-      </c>
-      <c r="Z4" t="s" s="15">
-        <v>66</v>
-      </c>
-      <c r="AA4" t="s" s="15">
-        <v>67</v>
-      </c>
-      <c r="AB4" t="s" s="15">
-        <v>68</v>
-      </c>
-      <c r="AC4" t="s" s="15">
-        <v>69</v>
-      </c>
-      <c r="AD4" t="s" s="15">
-        <v>70</v>
-      </c>
-      <c r="AE4" t="s" s="15">
-        <v>71</v>
-      </c>
-      <c r="AF4" t="s" s="15">
-        <v>72</v>
-      </c>
-      <c r="AG4" t="s" s="15">
-        <v>72</v>
-      </c>
-      <c r="AH4" t="s" s="15">
-        <v>73</v>
-      </c>
-      <c r="AI4" t="s" s="15">
-        <v>72</v>
-      </c>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="16"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="16"/>
+      <c r="AG4" s="16"/>
+      <c r="AH4" s="16"/>
+      <c r="AI4" s="16"/>
       <c r="AJ4" s="16"/>
       <c r="AK4" s="16"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="16"/>
       <c r="AN4" s="16"/>
       <c r="AO4" t="s" s="15">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="AP4" t="s" s="15">
-        <v>74</v>
-      </c>
-      <c r="AQ4" s="16"/>
+        <v>87</v>
+      </c>
+      <c r="AQ4" t="s" s="15">
+        <v>87</v>
+      </c>
       <c r="AR4" t="s" s="15">
-        <v>74</v>
-      </c>
-      <c r="AS4" t="s" s="15">
-        <v>75</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="AS4" s="16"/>
       <c r="AT4" s="16"/>
-      <c r="AU4" s="16"/>
+      <c r="AU4" t="s" s="15">
+        <v>87</v>
+      </c>
       <c r="AV4" s="16"/>
       <c r="AW4" s="16"/>
-      <c r="AX4" s="16"/>
+      <c r="AX4" t="s" s="15">
+        <v>88</v>
+      </c>
       <c r="AY4" s="16"/>
-      <c r="AZ4" t="s" s="15">
-        <v>76</v>
-      </c>
-      <c r="BA4" t="s" s="15">
-        <v>77</v>
-      </c>
-      <c r="BB4" t="s" s="15">
-        <v>75</v>
-      </c>
+      <c r="AZ4" s="16"/>
+      <c r="BA4" s="16"/>
+      <c r="BB4" s="16"/>
       <c r="BC4" s="16"/>
-    </row>
-    <row r="5" ht="74.35" customHeight="1">
-      <c r="A5" t="s" s="8">
-        <v>78</v>
-      </c>
+      <c r="BD4" s="16"/>
+      <c r="BE4" t="s" s="15">
+        <v>89</v>
+      </c>
+      <c r="BF4" t="s" s="15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" ht="19.35" customHeight="1">
+      <c r="A5" s="18"/>
       <c r="B5" s="14"/>
-      <c r="C5" t="s" s="15">
-        <v>79</v>
-      </c>
+      <c r="C5" s="16"/>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
@@ -2702,46 +3246,37 @@
       <c r="AH5" s="16"/>
       <c r="AI5" s="16"/>
       <c r="AJ5" s="16"/>
-      <c r="AK5" t="s" s="15">
-        <v>80</v>
-      </c>
-      <c r="AL5" t="s" s="15">
-        <v>80</v>
-      </c>
-      <c r="AM5" t="s" s="15">
-        <v>80</v>
-      </c>
-      <c r="AN5" t="s" s="15">
-        <v>80</v>
-      </c>
+      <c r="AK5" s="16"/>
+      <c r="AL5" s="16"/>
+      <c r="AM5" s="16"/>
+      <c r="AN5" s="16"/>
       <c r="AO5" s="16"/>
       <c r="AP5" s="16"/>
-      <c r="AQ5" t="s" s="15">
-        <v>80</v>
-      </c>
+      <c r="AQ5" s="16"/>
       <c r="AR5" s="16"/>
       <c r="AS5" s="16"/>
-      <c r="AT5" t="s" s="15">
-        <v>81</v>
-      </c>
+      <c r="AT5" s="16"/>
       <c r="AU5" s="16"/>
       <c r="AV5" s="16"/>
       <c r="AW5" s="16"/>
       <c r="AX5" s="16"/>
       <c r="AY5" s="16"/>
       <c r="AZ5" s="16"/>
-      <c r="BA5" t="s" s="15">
-        <v>82</v>
-      </c>
-      <c r="BB5" t="s" s="15">
-        <v>83</v>
-      </c>
+      <c r="BA5" s="16"/>
+      <c r="BB5" s="16"/>
       <c r="BC5" s="16"/>
-    </row>
-    <row r="6" ht="19.35" customHeight="1">
-      <c r="A6" s="17"/>
+      <c r="BD5" s="16"/>
+      <c r="BE5" s="16"/>
+      <c r="BF5" s="16"/>
+    </row>
+    <row r="6" ht="96.35" customHeight="1">
+      <c r="A6" t="s" s="8">
+        <v>91</v>
+      </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="16"/>
+      <c r="C6" t="s" s="15">
+        <v>92</v>
+      </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
@@ -2761,32 +3296,62 @@
       <c r="T6" s="16"/>
       <c r="U6" s="16"/>
       <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
+      <c r="W6" t="s" s="15">
+        <v>78</v>
+      </c>
       <c r="X6" s="16"/>
       <c r="Y6" s="16"/>
       <c r="Z6" s="16"/>
       <c r="AA6" s="16"/>
       <c r="AB6" s="16"/>
       <c r="AC6" s="16"/>
-      <c r="AD6" s="16"/>
+      <c r="AD6" t="s" s="15">
+        <v>93</v>
+      </c>
       <c r="AE6" s="16"/>
-      <c r="AF6" s="16"/>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="16"/>
-      <c r="AI6" s="16"/>
-      <c r="AJ6" s="16"/>
+      <c r="AF6" t="s" s="15">
+        <v>94</v>
+      </c>
+      <c r="AG6" t="s" s="15">
+        <v>95</v>
+      </c>
+      <c r="AH6" t="s" s="15">
+        <v>96</v>
+      </c>
+      <c r="AI6" s="15"/>
+      <c r="AJ6" t="s" s="15">
+        <v>97</v>
+      </c>
       <c r="AK6" s="16"/>
       <c r="AL6" s="16"/>
-      <c r="AM6" s="16"/>
-      <c r="AN6" s="16"/>
+      <c r="AM6" t="s" s="15">
+        <v>78</v>
+      </c>
+      <c r="AN6" t="s" s="15">
+        <v>98</v>
+      </c>
       <c r="AO6" s="16"/>
-      <c r="AP6" s="16"/>
-      <c r="AQ6" s="16"/>
-      <c r="AR6" s="16"/>
-      <c r="AS6" s="16"/>
-      <c r="AT6" s="16"/>
-      <c r="AU6" s="16"/>
-      <c r="AV6" s="16"/>
+      <c r="AP6" t="s" s="15">
+        <v>99</v>
+      </c>
+      <c r="AQ6" t="s" s="15">
+        <v>100</v>
+      </c>
+      <c r="AR6" t="s" s="15">
+        <v>100</v>
+      </c>
+      <c r="AS6" t="s" s="15">
+        <v>101</v>
+      </c>
+      <c r="AT6" t="s" s="15">
+        <v>102</v>
+      </c>
+      <c r="AU6" t="s" s="15">
+        <v>103</v>
+      </c>
+      <c r="AV6" t="s" s="15">
+        <v>104</v>
+      </c>
       <c r="AW6" s="16"/>
       <c r="AX6" s="16"/>
       <c r="AY6" s="16"/>
@@ -2794,15 +3359,18 @@
       <c r="BA6" s="16"/>
       <c r="BB6" s="16"/>
       <c r="BC6" s="16"/>
-    </row>
-    <row r="7" ht="96.35" customHeight="1">
+      <c r="BD6" s="16"/>
+      <c r="BE6" s="16"/>
+      <c r="BF6" t="s" s="15">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" ht="129.35" customHeight="1">
       <c r="A7" t="s" s="8">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B7" s="14"/>
-      <c r="C7" t="s" s="15">
-        <v>85</v>
-      </c>
+      <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
@@ -2810,7 +3378,9 @@
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="K7" t="s" s="15">
+        <v>105</v>
+      </c>
       <c r="L7" s="16"/>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
@@ -2824,74 +3394,69 @@
       <c r="V7" s="16"/>
       <c r="W7" s="16"/>
       <c r="X7" s="16"/>
-      <c r="Y7" t="s" s="15">
-        <v>86</v>
-      </c>
+      <c r="Y7" s="16"/>
       <c r="Z7" s="16"/>
-      <c r="AA7" t="s" s="15">
-        <v>87</v>
-      </c>
-      <c r="AB7" t="s" s="15">
-        <v>88</v>
-      </c>
-      <c r="AC7" t="s" s="15">
-        <v>89</v>
-      </c>
-      <c r="AD7" t="s" s="15">
-        <v>72</v>
-      </c>
-      <c r="AE7" t="s" s="15">
-        <v>90</v>
-      </c>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="16"/>
       <c r="AF7" s="16"/>
-      <c r="AG7" s="16"/>
-      <c r="AH7" s="16"/>
-      <c r="AI7" t="s" s="15">
-        <v>72</v>
-      </c>
+      <c r="AG7" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="AH7" t="s" s="15">
+        <v>106</v>
+      </c>
+      <c r="AI7" s="15"/>
       <c r="AJ7" t="s" s="15">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="AK7" s="16"/>
-      <c r="AL7" t="s" s="15">
-        <v>92</v>
-      </c>
-      <c r="AM7" t="s" s="15">
-        <v>93</v>
-      </c>
-      <c r="AN7" t="s" s="15">
-        <v>93</v>
-      </c>
+      <c r="AL7" s="16"/>
+      <c r="AM7" s="16"/>
+      <c r="AN7" s="16"/>
       <c r="AO7" t="s" s="15">
-        <v>94</v>
-      </c>
-      <c r="AP7" t="s" s="15">
-        <v>95</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="AP7" s="16"/>
       <c r="AQ7" t="s" s="15">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="AR7" t="s" s="15">
-        <v>97</v>
-      </c>
-      <c r="AS7" s="16"/>
+        <v>110</v>
+      </c>
+      <c r="AS7" t="s" s="15">
+        <v>111</v>
+      </c>
       <c r="AT7" s="16"/>
       <c r="AU7" s="16"/>
       <c r="AV7" s="16"/>
       <c r="AW7" s="16"/>
       <c r="AX7" s="16"/>
       <c r="AY7" s="16"/>
-      <c r="AZ7" s="16"/>
-      <c r="BA7" s="16"/>
+      <c r="AZ7" t="s" s="15">
+        <v>112</v>
+      </c>
+      <c r="BA7" t="s" s="15">
+        <v>113</v>
+      </c>
       <c r="BB7" t="s" s="15">
-        <v>75</v>
-      </c>
-      <c r="BC7" s="16"/>
-    </row>
-    <row r="8" ht="129.35" customHeight="1">
-      <c r="A8" t="s" s="8">
-        <v>78</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="BC7" t="s" s="15">
+        <v>115</v>
+      </c>
+      <c r="BD7" s="16"/>
+      <c r="BE7" t="s" s="15">
+        <v>116</v>
+      </c>
+      <c r="BF7" t="s" s="15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" ht="19.35" customHeight="1">
+      <c r="A8" s="18"/>
       <c r="B8" s="14"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
@@ -2901,9 +3466,7 @@
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
-      <c r="K8" t="s" s="15">
-        <v>98</v>
-      </c>
+      <c r="K8" s="16"/>
       <c r="L8" s="16"/>
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
@@ -2920,63 +3483,42 @@
       <c r="Y8" s="16"/>
       <c r="Z8" s="16"/>
       <c r="AA8" s="16"/>
-      <c r="AB8" t="s" s="15">
-        <v>71</v>
-      </c>
-      <c r="AC8" t="s" s="15">
-        <v>99</v>
-      </c>
+      <c r="AB8" s="16"/>
+      <c r="AC8" s="16"/>
       <c r="AD8" s="16"/>
-      <c r="AE8" t="s" s="15">
-        <v>100</v>
-      </c>
+      <c r="AE8" s="16"/>
       <c r="AF8" s="16"/>
       <c r="AG8" s="16"/>
       <c r="AH8" s="16"/>
       <c r="AI8" s="16"/>
       <c r="AJ8" s="16"/>
-      <c r="AK8" t="s" s="15">
-        <v>101</v>
-      </c>
+      <c r="AK8" s="16"/>
       <c r="AL8" s="16"/>
-      <c r="AM8" t="s" s="15">
-        <v>102</v>
-      </c>
-      <c r="AN8" t="s" s="15">
-        <v>103</v>
-      </c>
-      <c r="AO8" t="s" s="15">
-        <v>104</v>
-      </c>
+      <c r="AM8" s="16"/>
+      <c r="AN8" s="16"/>
+      <c r="AO8" s="16"/>
       <c r="AP8" s="16"/>
       <c r="AQ8" s="16"/>
       <c r="AR8" s="16"/>
       <c r="AS8" s="16"/>
       <c r="AT8" s="16"/>
       <c r="AU8" s="16"/>
-      <c r="AV8" t="s" s="15">
-        <v>105</v>
-      </c>
-      <c r="AW8" t="s" s="15">
-        <v>106</v>
-      </c>
-      <c r="AX8" t="s" s="15">
-        <v>107</v>
-      </c>
-      <c r="AY8" t="s" s="15">
-        <v>108</v>
-      </c>
+      <c r="AV8" s="16"/>
+      <c r="AW8" s="16"/>
+      <c r="AX8" s="16"/>
+      <c r="AY8" s="16"/>
       <c r="AZ8" s="16"/>
-      <c r="BA8" t="s" s="15">
-        <v>109</v>
-      </c>
-      <c r="BB8" t="s" s="15">
-        <v>110</v>
-      </c>
+      <c r="BA8" s="16"/>
+      <c r="BB8" s="16"/>
       <c r="BC8" s="16"/>
-    </row>
-    <row r="9" ht="19.35" customHeight="1">
-      <c r="A9" s="17"/>
+      <c r="BD8" s="16"/>
+      <c r="BE8" s="16"/>
+      <c r="BF8" s="16"/>
+    </row>
+    <row r="9" ht="30.35" customHeight="1">
+      <c r="A9" t="s" s="8">
+        <v>118</v>
+      </c>
       <c r="B9" s="14"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
@@ -2998,7 +3540,9 @@
       <c r="T9" s="16"/>
       <c r="U9" s="16"/>
       <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
+      <c r="W9" t="s" s="15">
+        <v>79</v>
+      </c>
       <c r="X9" s="16"/>
       <c r="Y9" s="16"/>
       <c r="Z9" s="16"/>
@@ -3007,9 +3551,13 @@
       <c r="AC9" s="16"/>
       <c r="AD9" s="16"/>
       <c r="AE9" s="16"/>
-      <c r="AF9" s="16"/>
+      <c r="AF9" t="s" s="15">
+        <v>92</v>
+      </c>
       <c r="AG9" s="16"/>
-      <c r="AH9" s="16"/>
+      <c r="AH9" t="s" s="15">
+        <v>119</v>
+      </c>
       <c r="AI9" s="16"/>
       <c r="AJ9" s="16"/>
       <c r="AK9" s="16"/>
@@ -3031,11 +3579,12 @@
       <c r="BA9" s="16"/>
       <c r="BB9" s="16"/>
       <c r="BC9" s="16"/>
-    </row>
-    <row r="10" ht="30.35" customHeight="1">
-      <c r="A10" t="s" s="8">
-        <v>111</v>
-      </c>
+      <c r="BD9" s="16"/>
+      <c r="BE9" s="16"/>
+      <c r="BF9" s="16"/>
+    </row>
+    <row r="10" ht="19.35" customHeight="1">
+      <c r="A10" s="18"/>
       <c r="B10" s="14"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
@@ -3061,16 +3610,10 @@
       <c r="X10" s="16"/>
       <c r="Y10" s="16"/>
       <c r="Z10" s="16"/>
-      <c r="AA10" t="s" s="15">
-        <v>85</v>
-      </c>
+      <c r="AA10" s="16"/>
       <c r="AB10" s="16"/>
-      <c r="AC10" t="s" s="15">
-        <v>112</v>
-      </c>
-      <c r="AD10" t="s" s="15">
-        <v>71</v>
-      </c>
+      <c r="AC10" s="16"/>
+      <c r="AD10" s="16"/>
       <c r="AE10" s="16"/>
       <c r="AF10" s="16"/>
       <c r="AG10" s="16"/>
@@ -3096,14 +3639,27 @@
       <c r="BA10" s="16"/>
       <c r="BB10" s="16"/>
       <c r="BC10" s="16"/>
-    </row>
-    <row r="11" ht="19.35" customHeight="1">
-      <c r="A11" s="17"/>
+      <c r="BD10" s="16"/>
+      <c r="BE10" s="16"/>
+      <c r="BF10" s="16"/>
+    </row>
+    <row r="11" ht="261.35" customHeight="1">
+      <c r="A11" t="s" s="8">
+        <v>120</v>
+      </c>
       <c r="B11" s="14"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="C11" t="s" s="15">
+        <v>121</v>
+      </c>
+      <c r="D11" t="s" s="15">
+        <v>122</v>
+      </c>
+      <c r="E11" t="s" s="15">
+        <v>123</v>
+      </c>
+      <c r="F11" t="s" s="19">
+        <v>124</v>
+      </c>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
@@ -3111,66 +3667,93 @@
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
+      <c r="N11" t="s" s="19">
+        <v>125</v>
+      </c>
+      <c r="O11" s="19"/>
       <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
+      <c r="Q11" t="s" s="15">
+        <v>126</v>
+      </c>
       <c r="R11" s="16"/>
       <c r="S11" s="16"/>
       <c r="T11" s="16"/>
       <c r="U11" s="16"/>
       <c r="V11" s="16"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="16"/>
-      <c r="Y11" s="16"/>
-      <c r="Z11" s="16"/>
-      <c r="AA11" s="16"/>
-      <c r="AB11" s="16"/>
+      <c r="W11" t="s" s="15">
+        <v>127</v>
+      </c>
+      <c r="X11" t="s" s="15">
+        <v>128</v>
+      </c>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+      <c r="AB11" t="s" s="15">
+        <v>129</v>
+      </c>
       <c r="AC11" s="16"/>
-      <c r="AD11" s="16"/>
-      <c r="AE11" s="16"/>
-      <c r="AF11" s="16"/>
-      <c r="AG11" s="16"/>
-      <c r="AH11" s="16"/>
-      <c r="AI11" s="16"/>
-      <c r="AJ11" s="16"/>
-      <c r="AK11" s="16"/>
-      <c r="AL11" s="16"/>
+      <c r="AD11" t="s" s="15">
+        <v>130</v>
+      </c>
+      <c r="AE11" t="s" s="15">
+        <v>131</v>
+      </c>
+      <c r="AF11" t="s" s="15">
+        <v>132</v>
+      </c>
+      <c r="AG11" t="s" s="15">
+        <v>133</v>
+      </c>
+      <c r="AH11" t="s" s="15">
+        <v>134</v>
+      </c>
+      <c r="AI11" t="s" s="15">
+        <v>135</v>
+      </c>
+      <c r="AJ11" t="s" s="15">
+        <v>136</v>
+      </c>
+      <c r="AK11" t="s" s="15">
+        <v>137</v>
+      </c>
+      <c r="AL11" t="s" s="15">
+        <v>138</v>
+      </c>
       <c r="AM11" s="16"/>
       <c r="AN11" s="16"/>
-      <c r="AO11" s="16"/>
+      <c r="AO11" t="s" s="15">
+        <v>139</v>
+      </c>
       <c r="AP11" s="16"/>
       <c r="AQ11" s="16"/>
       <c r="AR11" s="16"/>
       <c r="AS11" s="16"/>
-      <c r="AT11" s="16"/>
+      <c r="AT11" t="s" s="15">
+        <v>140</v>
+      </c>
       <c r="AU11" s="16"/>
       <c r="AV11" s="16"/>
       <c r="AW11" s="16"/>
-      <c r="AX11" s="16"/>
+      <c r="AX11" t="s" s="15">
+        <v>141</v>
+      </c>
       <c r="AY11" s="16"/>
       <c r="AZ11" s="16"/>
       <c r="BA11" s="16"/>
       <c r="BB11" s="16"/>
       <c r="BC11" s="16"/>
-    </row>
-    <row r="12" ht="261.35" customHeight="1">
-      <c r="A12" t="s" s="8">
-        <v>113</v>
-      </c>
+      <c r="BD11" s="16"/>
+      <c r="BE11" s="16"/>
+      <c r="BF11" s="16"/>
+    </row>
+    <row r="12" ht="19.35" customHeight="1">
+      <c r="A12" s="18"/>
       <c r="B12" s="14"/>
-      <c r="C12" t="s" s="15">
-        <v>114</v>
-      </c>
-      <c r="D12" t="s" s="15">
-        <v>115</v>
-      </c>
-      <c r="E12" t="s" s="15">
-        <v>116</v>
-      </c>
-      <c r="F12" t="s" s="18">
-        <v>117</v>
-      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
@@ -3178,73 +3761,39 @@
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
       <c r="M12" s="16"/>
-      <c r="N12" t="s" s="18">
-        <v>118</v>
-      </c>
-      <c r="O12" t="s" s="15">
-        <v>119</v>
-      </c>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
       <c r="P12" s="16"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
       <c r="S12" s="16"/>
       <c r="T12" s="16"/>
       <c r="U12" s="16"/>
-      <c r="V12" t="s" s="15">
-        <v>120</v>
-      </c>
+      <c r="V12" s="16"/>
       <c r="W12" s="16"/>
-      <c r="X12" t="s" s="15">
-        <v>121</v>
-      </c>
-      <c r="Y12" t="s" s="15">
-        <v>122</v>
-      </c>
-      <c r="Z12" t="s" s="15">
-        <v>123</v>
-      </c>
-      <c r="AA12" t="s" s="15">
-        <v>124</v>
-      </c>
-      <c r="AB12" t="s" s="15">
-        <v>125</v>
-      </c>
-      <c r="AC12" t="s" s="15">
-        <v>126</v>
-      </c>
-      <c r="AD12" t="s" s="15">
-        <v>127</v>
-      </c>
-      <c r="AE12" t="s" s="15">
-        <v>128</v>
-      </c>
-      <c r="AF12" t="s" s="15">
-        <v>129</v>
-      </c>
-      <c r="AG12" t="s" s="15">
-        <v>130</v>
-      </c>
-      <c r="AH12" t="s" s="15">
-        <v>131</v>
-      </c>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="16"/>
+      <c r="AA12" s="16"/>
+      <c r="AB12" s="16"/>
+      <c r="AC12" s="16"/>
+      <c r="AD12" s="16"/>
+      <c r="AE12" s="16"/>
+      <c r="AF12" s="16"/>
+      <c r="AG12" s="16"/>
+      <c r="AH12" s="16"/>
       <c r="AI12" s="16"/>
       <c r="AJ12" s="16"/>
-      <c r="AK12" t="s" s="15">
-        <v>132</v>
-      </c>
+      <c r="AK12" s="16"/>
       <c r="AL12" s="16"/>
       <c r="AM12" s="16"/>
       <c r="AN12" s="16"/>
       <c r="AO12" s="16"/>
-      <c r="AP12" t="s" s="15">
-        <v>133</v>
-      </c>
+      <c r="AP12" s="16"/>
       <c r="AQ12" s="16"/>
       <c r="AR12" s="16"/>
       <c r="AS12" s="16"/>
-      <c r="AT12" t="s" s="15">
-        <v>134</v>
-      </c>
+      <c r="AT12" s="16"/>
       <c r="AU12" s="16"/>
       <c r="AV12" s="16"/>
       <c r="AW12" s="16"/>
@@ -3254,467 +3803,1526 @@
       <c r="BA12" s="16"/>
       <c r="BB12" s="16"/>
       <c r="BC12" s="16"/>
+      <c r="BD12" s="16"/>
+      <c r="BE12" s="16"/>
+      <c r="BF12" s="16"/>
     </row>
     <row r="13" ht="19.35" customHeight="1">
-      <c r="A13" s="17"/>
+      <c r="A13" t="s" s="8">
+        <v>142</v>
+      </c>
       <c r="B13" s="14"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="G13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="H13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="I13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="J13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K13" s="15"/>
+      <c r="L13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="M13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="N13" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="O13" s="15"/>
+      <c r="P13" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="Q13" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="R13" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="S13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="T13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="U13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="V13" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="W13" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="X13" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="AC13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="AD13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="AE13" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="AF13" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="AG13" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="AH13" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="AI13" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="AJ13" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="AK13" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="AL13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="AM13" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="AN13" s="16"/>
+      <c r="AO13" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="AP13" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="AQ13" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="AR13" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="AS13" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="AT13" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="AU13" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="AV13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="AW13" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="AX13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="AY13" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="AZ13" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="BA13" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="BB13" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="BC13" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="BD13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="BE13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="BF13" t="s" s="15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" ht="19.35" customHeight="1">
+      <c r="A14" t="s" s="8">
+        <v>146</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="T14" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="U14" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="AC14" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="15"/>
+      <c r="AF14" s="15"/>
+      <c r="AG14" s="15"/>
+      <c r="AH14" s="15"/>
+      <c r="AI14" s="15"/>
+      <c r="AJ14" s="15"/>
+      <c r="AK14" s="15"/>
+      <c r="AL14" s="15"/>
+      <c r="AM14" s="15"/>
+      <c r="AN14" s="16"/>
+      <c r="AO14" s="15"/>
+      <c r="AP14" s="15"/>
+      <c r="AQ14" s="15"/>
+      <c r="AR14" s="15"/>
+      <c r="AS14" s="15"/>
+      <c r="AT14" s="15"/>
+      <c r="AU14" s="15"/>
+      <c r="AV14" s="15"/>
+      <c r="AW14" s="15"/>
+      <c r="AX14" s="15"/>
+      <c r="AY14" s="15"/>
+      <c r="AZ14" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="BA14" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="BB14" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="BC14" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="BD14" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="BE14" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="BF14" t="s" s="15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" ht="19.35" customHeight="1">
+      <c r="A15" s="18"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
+      <c r="W15" s="16"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="16"/>
+      <c r="Z15" s="16"/>
+      <c r="AA15" s="16"/>
+      <c r="AB15" s="16"/>
+      <c r="AC15" s="16"/>
+      <c r="AD15" s="16"/>
+      <c r="AE15" s="16"/>
+      <c r="AF15" s="16"/>
+      <c r="AG15" s="16"/>
+      <c r="AH15" s="16"/>
+      <c r="AI15" s="16"/>
+      <c r="AJ15" s="16"/>
+      <c r="AK15" s="16"/>
+      <c r="AL15" s="16"/>
+      <c r="AM15" s="16"/>
+      <c r="AN15" s="16"/>
+      <c r="AO15" s="16"/>
+      <c r="AP15" s="16"/>
+      <c r="AQ15" s="16"/>
+      <c r="AR15" s="16"/>
+      <c r="AS15" s="16"/>
+      <c r="AT15" s="16"/>
+      <c r="AU15" s="16"/>
+      <c r="AV15" s="16"/>
+      <c r="AW15" s="16"/>
+      <c r="AX15" s="16"/>
+      <c r="AY15" s="16"/>
+      <c r="AZ15" s="16"/>
+      <c r="BA15" s="16"/>
+      <c r="BB15" s="16"/>
+      <c r="BC15" s="16"/>
+      <c r="BD15" s="16"/>
+      <c r="BE15" s="16"/>
+      <c r="BF15" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="K1:AC1"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="AD1:AH1"/>
+    <mergeCell ref="AO1:AQ1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="AG2" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="AH2" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="O3" r:id="rId3" location="" tooltip="" display=""/>
+    <hyperlink ref="P3" r:id="rId4" location="" tooltip="" display=""/>
+    <hyperlink ref="Q3" r:id="rId5" location="" tooltip="" display=""/>
+    <hyperlink ref="V3" r:id="rId6" location="" tooltip="" display=""/>
+    <hyperlink ref="X3" r:id="rId7" location="" tooltip="" display=""/>
+    <hyperlink ref="Y3" r:id="rId8" location="" tooltip="" display=""/>
+    <hyperlink ref="Z3" r:id="rId9" location="" tooltip="" display=""/>
+    <hyperlink ref="AA3" r:id="rId10" location="" tooltip="" display=""/>
+    <hyperlink ref="BE7" r:id="rId11" location="" tooltip="" display=""/>
+    <hyperlink ref="X11" r:id="rId12" location="" tooltip="" display=""/>
+  </hyperlinks>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="19.6" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="19.6016" style="20" customWidth="1"/>
+    <col min="2" max="2" width="19.6016" style="20" customWidth="1"/>
+    <col min="3" max="3" width="19.6016" style="20" customWidth="1"/>
+    <col min="4" max="4" width="19.6016" style="20" customWidth="1"/>
+    <col min="5" max="5" width="19.6016" style="20" customWidth="1"/>
+    <col min="6" max="6" width="19.6016" style="20" customWidth="1"/>
+    <col min="7" max="7" width="19.6016" style="20" customWidth="1"/>
+    <col min="8" max="8" width="19.6016" style="20" customWidth="1"/>
+    <col min="9" max="9" width="19.6016" style="20" customWidth="1"/>
+    <col min="10" max="10" width="19.6016" style="20" customWidth="1"/>
+    <col min="11" max="11" width="19.6016" style="20" customWidth="1"/>
+    <col min="12" max="256" width="19.6016" style="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="25" customHeight="1">
+      <c r="A1" t="s" s="21">
+        <v>147</v>
+      </c>
+      <c r="B1" t="s" s="22">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s" s="23">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s" s="23">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s" s="23">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s" s="23">
+        <v>91</v>
+      </c>
+      <c r="G1" t="s" s="23">
+        <v>85</v>
+      </c>
+      <c r="H1" t="s" s="23">
+        <v>118</v>
+      </c>
+      <c r="I1" t="s" s="23">
+        <v>120</v>
+      </c>
+      <c r="J1" t="s" s="23">
+        <v>142</v>
+      </c>
+      <c r="K1" t="s" s="23">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" ht="25" customHeight="1">
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" t="s" s="26">
+        <v>13</v>
+      </c>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+    </row>
+    <row r="3" ht="201" customHeight="1">
+      <c r="A3" s="24"/>
+      <c r="B3" s="28"/>
+      <c r="C3" t="s" s="29">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s" s="15">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s" s="15">
+        <v>86</v>
+      </c>
+      <c r="F3" t="s" s="15">
+        <v>92</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" t="s" s="15">
+        <v>121</v>
+      </c>
+      <c r="J3" s="15"/>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" ht="80" customHeight="1">
+      <c r="A4" s="24"/>
+      <c r="B4" t="s" s="30">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s" s="29">
+        <v>15</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" t="s" s="15">
+        <v>122</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" ht="58" customHeight="1">
+      <c r="A5" s="24"/>
+      <c r="B5" s="31"/>
+      <c r="C5" t="s" s="29">
+        <v>16</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" t="s" s="15">
+        <v>123</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" ht="90.7" customHeight="1">
+      <c r="A6" s="24"/>
+      <c r="B6" s="31"/>
+      <c r="C6" t="s" s="32">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s" s="15">
+        <v>51</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" t="s" s="19">
+        <v>124</v>
+      </c>
+      <c r="J6" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" ht="25" customHeight="1">
+      <c r="A7" s="24"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="33"/>
+      <c r="D7" t="s" s="15">
+        <v>52</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" ht="58" customHeight="1">
+      <c r="A8" s="24"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="33"/>
+      <c r="D8" t="s" s="15">
+        <v>53</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" ht="36" customHeight="1">
+      <c r="A9" s="24"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="33"/>
+      <c r="D9" t="s" s="15">
+        <v>54</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" ht="80" customHeight="1">
+      <c r="A10" s="24"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="33"/>
+      <c r="D10" t="s" s="15">
+        <v>55</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" ht="14" customHeight="1">
+      <c r="A11" s="24"/>
+      <c r="B11" t="s" s="30">
+        <v>2</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" t="s" s="15">
+        <v>105</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" ht="36" customHeight="1">
+      <c r="A12" s="24"/>
+      <c r="B12" s="28"/>
+      <c r="C12" t="s" s="29">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s" s="15">
+        <v>56</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" ht="14" customHeight="1">
+      <c r="A13" s="24"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="33"/>
+      <c r="D13" t="s" s="15">
+        <v>57</v>
+      </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
-      <c r="U13" s="16"/>
-      <c r="V13" s="16"/>
-      <c r="W13" s="16"/>
-      <c r="X13" s="16"/>
-      <c r="Y13" s="16"/>
-      <c r="Z13" s="16"/>
-      <c r="AA13" s="16"/>
-      <c r="AB13" s="16"/>
-      <c r="AC13" s="16"/>
-      <c r="AD13" s="16"/>
-      <c r="AE13" s="16"/>
-      <c r="AF13" s="16"/>
-      <c r="AG13" s="16"/>
-      <c r="AH13" s="16"/>
-      <c r="AI13" s="16"/>
-      <c r="AJ13" s="16"/>
-      <c r="AK13" s="16"/>
-      <c r="AL13" s="16"/>
-      <c r="AM13" s="16"/>
-      <c r="AN13" s="16"/>
-      <c r="AO13" s="16"/>
-      <c r="AP13" s="16"/>
-      <c r="AQ13" s="16"/>
-      <c r="AR13" s="16"/>
-      <c r="AS13" s="16"/>
-      <c r="AT13" s="16"/>
-      <c r="AU13" s="16"/>
-      <c r="AV13" s="16"/>
-      <c r="AW13" s="16"/>
-      <c r="AX13" s="16"/>
-      <c r="AY13" s="16"/>
-      <c r="AZ13" s="16"/>
-      <c r="BA13" s="16"/>
-      <c r="BB13" s="16"/>
-      <c r="BC13" s="16"/>
-    </row>
-    <row r="14" ht="19.35" customHeight="1">
-      <c r="A14" t="s" s="8">
-        <v>135</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" t="s" s="15">
-        <v>136</v>
+      <c r="J13" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" ht="123.7" customHeight="1">
+      <c r="A14" s="24"/>
+      <c r="B14" s="28"/>
+      <c r="C14" t="s" s="29">
+        <v>19</v>
       </c>
       <c r="D14" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="E14" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="F14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="G14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="H14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="I14" t="s" s="15">
-        <v>136</v>
+        <v>57</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" t="s" s="19">
+        <v>125</v>
       </c>
       <c r="J14" t="s" s="15">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="K14" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="L14" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="M14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="N14" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="O14" t="s" s="15">
-        <v>138</v>
-      </c>
-      <c r="P14" t="s" s="15">
-        <v>138</v>
-      </c>
-      <c r="Q14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="R14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="S14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="T14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="U14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="V14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="W14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="X14" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="Y14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="Z14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="AA14" t="s" s="15">
-        <v>138</v>
-      </c>
-      <c r="AB14" t="s" s="15">
-        <v>138</v>
-      </c>
-      <c r="AC14" t="s" s="15">
-        <v>138</v>
-      </c>
-      <c r="AD14" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AE14" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AF14" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AG14" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AH14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="AI14" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AJ14" s="16"/>
-      <c r="AK14" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AL14" t="s" s="15">
-        <v>138</v>
-      </c>
-      <c r="AM14" t="s" s="15">
-        <v>138</v>
-      </c>
-      <c r="AN14" t="s" s="15">
-        <v>138</v>
-      </c>
-      <c r="AO14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="AP14" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AQ14" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AR14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="AS14" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AT14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="AU14" t="s" s="15">
-        <v>71</v>
-      </c>
-      <c r="AV14" t="s" s="15">
-        <v>71</v>
-      </c>
-      <c r="AW14" t="s" s="15">
-        <v>71</v>
-      </c>
-      <c r="AX14" t="s" s="15">
-        <v>71</v>
-      </c>
-      <c r="AY14" t="s" s="15">
-        <v>71</v>
-      </c>
-      <c r="AZ14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="BA14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="BB14" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="BC14" s="16"/>
-    </row>
-    <row r="15" ht="19.35" customHeight="1">
-      <c r="A15" t="s" s="8">
-        <v>139</v>
-      </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="16"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" ht="36" customHeight="1">
+      <c r="A15" s="35"/>
+      <c r="B15" s="31"/>
+      <c r="C15" t="s" s="29">
+        <v>21</v>
+      </c>
       <c r="D15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="E15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="F15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="G15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="H15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="I15" t="s" s="15">
-        <v>136</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
       <c r="J15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="K15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="L15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="M15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="N15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="O15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="P15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="Q15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="R15" t="s" s="15">
-        <v>138</v>
-      </c>
-      <c r="S15" t="s" s="15">
-        <v>138</v>
-      </c>
-      <c r="T15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="U15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="V15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="W15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="X15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="Y15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="Z15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="AA15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AB15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AC15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AD15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AE15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="AF15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="AG15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="AH15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AI15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AJ15" s="16"/>
-      <c r="AK15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="AL15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AM15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AN15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AO15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="AP15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="AQ15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AR15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AS15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AT15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AU15" t="s" s="15">
-        <v>137</v>
-      </c>
-      <c r="AV15" t="s" s="15">
-        <v>71</v>
-      </c>
-      <c r="AW15" t="s" s="15">
-        <v>71</v>
-      </c>
-      <c r="AX15" t="s" s="15">
-        <v>71</v>
-      </c>
-      <c r="AY15" t="s" s="15">
-        <v>71</v>
-      </c>
-      <c r="AZ15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="BA15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="BB15" t="s" s="15">
-        <v>136</v>
-      </c>
-      <c r="BC15" s="16"/>
-    </row>
-    <row r="16" ht="19.35" customHeight="1">
-      <c r="A16" s="17"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+        <v>144</v>
+      </c>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" ht="58" customHeight="1">
+      <c r="A16" s="35"/>
+      <c r="B16" s="31"/>
+      <c r="C16" t="s" s="29">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s" s="15">
+        <v>149</v>
+      </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="16"/>
-      <c r="T16" s="16"/>
-      <c r="U16" s="16"/>
-      <c r="V16" s="16"/>
-      <c r="W16" s="16"/>
-      <c r="X16" s="16"/>
-      <c r="Y16" s="16"/>
-      <c r="Z16" s="16"/>
-      <c r="AA16" s="16"/>
-      <c r="AB16" s="16"/>
-      <c r="AC16" s="16"/>
-      <c r="AD16" s="16"/>
-      <c r="AE16" s="16"/>
-      <c r="AF16" s="16"/>
-      <c r="AG16" s="16"/>
-      <c r="AH16" s="16"/>
-      <c r="AI16" s="16"/>
-      <c r="AJ16" s="16"/>
-      <c r="AK16" s="16"/>
-      <c r="AL16" s="16"/>
-      <c r="AM16" s="16"/>
-      <c r="AN16" s="16"/>
-      <c r="AO16" s="16"/>
-      <c r="AP16" s="16"/>
-      <c r="AQ16" s="16"/>
-      <c r="AR16" s="16"/>
-      <c r="AS16" s="16"/>
-      <c r="AT16" s="16"/>
-      <c r="AU16" s="16"/>
-      <c r="AV16" s="16"/>
-      <c r="AW16" s="16"/>
-      <c r="AX16" s="16"/>
-      <c r="AY16" s="16"/>
-      <c r="AZ16" s="16"/>
-      <c r="BA16" s="16"/>
-      <c r="BB16" s="16"/>
-      <c r="BC16" s="16"/>
+      <c r="I16" t="s" s="15">
+        <v>126</v>
+      </c>
+      <c r="J16" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" ht="36" customHeight="1">
+      <c r="A17" s="24"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="33"/>
+      <c r="D17" t="s" s="15">
+        <v>61</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" ht="14" customHeight="1">
+      <c r="A18" s="24"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="33"/>
+      <c r="D18" t="s" s="15">
+        <v>62</v>
+      </c>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K18" t="s" s="15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" ht="14" customHeight="1">
+      <c r="A19" s="24"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="33"/>
+      <c r="D19" t="s" s="15">
+        <v>63</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K19" t="s" s="15">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" ht="14" customHeight="1">
+      <c r="A20" s="24"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="33"/>
+      <c r="D20" t="s" s="15">
+        <v>64</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K20" t="s" s="15">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" ht="58" customHeight="1">
+      <c r="A21" s="24"/>
+      <c r="B21" s="28"/>
+      <c r="C21" t="s" s="29">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s" s="15">
+        <v>65</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="K21" s="15"/>
+    </row>
+    <row r="22" ht="102" customHeight="1">
+      <c r="A22" s="35"/>
+      <c r="B22" s="28"/>
+      <c r="C22" t="s" s="29">
+        <v>150</v>
+      </c>
+      <c r="D22" t="s" s="15">
+        <v>71</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" t="s" s="15">
+        <v>129</v>
+      </c>
+      <c r="J22" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K22" t="s" s="15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" ht="47" customHeight="1">
+      <c r="A23" s="24"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="33"/>
+      <c r="D23" t="s" s="15">
+        <v>72</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K23" t="s" s="15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" ht="36" customHeight="1">
+      <c r="A24" s="24"/>
+      <c r="B24" t="s" s="30">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s" s="29">
+        <v>151</v>
+      </c>
+      <c r="D24" t="s" s="15">
+        <v>57</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" t="s" s="15">
+        <v>152</v>
+      </c>
+      <c r="J24" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="K24" s="15"/>
+    </row>
+    <row r="25" ht="69" customHeight="1">
+      <c r="A25" s="24"/>
+      <c r="B25" s="31"/>
+      <c r="C25" t="s" s="29">
+        <v>153</v>
+      </c>
+      <c r="D25" t="s" s="15">
+        <v>73</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" t="s" s="15">
+        <v>93</v>
+      </c>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" t="s" s="15">
+        <v>130</v>
+      </c>
+      <c r="J25" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K25" s="15"/>
+    </row>
+    <row r="26" ht="58" customHeight="1">
+      <c r="A26" s="24"/>
+      <c r="B26" s="31"/>
+      <c r="C26" t="s" s="29">
+        <v>31</v>
+      </c>
+      <c r="D26" t="s" s="15">
+        <v>74</v>
+      </c>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" t="s" s="15">
+        <v>131</v>
+      </c>
+      <c r="J26" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="K26" s="15"/>
+    </row>
+    <row r="27" ht="36" customHeight="1">
+      <c r="A27" s="24"/>
+      <c r="B27" s="31"/>
+      <c r="C27" t="s" s="29">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s" s="15">
+        <v>75</v>
+      </c>
+      <c r="E27" s="16"/>
+      <c r="F27" t="s" s="15">
+        <v>94</v>
+      </c>
+      <c r="G27" s="16"/>
+      <c r="H27" t="s" s="15">
+        <v>92</v>
+      </c>
+      <c r="I27" t="s" s="15">
+        <v>132</v>
+      </c>
+      <c r="J27" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="K27" s="15"/>
+    </row>
+    <row r="28" ht="36" customHeight="1">
+      <c r="A28" s="24"/>
+      <c r="B28" s="31"/>
+      <c r="C28" t="s" s="29">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s" s="15">
+        <v>76</v>
+      </c>
+      <c r="E28" s="16"/>
+      <c r="F28" t="s" s="15">
+        <v>95</v>
+      </c>
+      <c r="G28" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="H28" s="16"/>
+      <c r="I28" t="s" s="15">
+        <v>133</v>
+      </c>
+      <c r="J28" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="K28" s="15"/>
+    </row>
+    <row r="29" ht="36" customHeight="1">
+      <c r="A29" s="24"/>
+      <c r="B29" s="31"/>
+      <c r="C29" t="s" s="29">
+        <v>34</v>
+      </c>
+      <c r="D29" t="s" s="15">
+        <v>77</v>
+      </c>
+      <c r="E29" s="16"/>
+      <c r="F29" t="s" s="15">
+        <v>96</v>
+      </c>
+      <c r="G29" t="s" s="15">
+        <v>106</v>
+      </c>
+      <c r="H29" t="s" s="15">
+        <v>119</v>
+      </c>
+      <c r="I29" t="s" s="15">
+        <v>134</v>
+      </c>
+      <c r="J29" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="K29" s="15"/>
+    </row>
+    <row r="30" ht="47" customHeight="1">
+      <c r="A30" s="24"/>
+      <c r="B30" s="31"/>
+      <c r="C30" t="s" s="29">
+        <v>24</v>
+      </c>
+      <c r="D30" t="s" s="15">
+        <v>66</v>
+      </c>
+      <c r="E30" s="16"/>
+      <c r="F30" t="s" s="15">
+        <v>78</v>
+      </c>
+      <c r="G30" s="16"/>
+      <c r="H30" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="I30" t="s" s="15">
+        <v>127</v>
+      </c>
+      <c r="J30" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="K30" s="15"/>
+    </row>
+    <row r="31" ht="234" customHeight="1">
+      <c r="A31" s="35"/>
+      <c r="B31" t="s" s="30">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s" s="29">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s" s="15">
+        <v>78</v>
+      </c>
+      <c r="E31" s="16"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="16"/>
+      <c r="I31" t="s" s="15">
+        <v>135</v>
+      </c>
+      <c r="J31" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="K31" s="15"/>
+    </row>
+    <row r="32" ht="113" customHeight="1">
+      <c r="A32" s="24"/>
+      <c r="B32" s="31"/>
+      <c r="C32" t="s" s="29">
+        <v>36</v>
+      </c>
+      <c r="D32" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="E32" s="16"/>
+      <c r="F32" t="s" s="15">
+        <v>97</v>
+      </c>
+      <c r="G32" t="s" s="15">
+        <v>107</v>
+      </c>
+      <c r="H32" s="16"/>
+      <c r="I32" t="s" s="15">
+        <v>136</v>
+      </c>
+      <c r="J32" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="K32" s="15"/>
+    </row>
+    <row r="33" ht="102" customHeight="1">
+      <c r="A33" s="24"/>
+      <c r="B33" s="31"/>
+      <c r="C33" t="s" s="29">
+        <v>37</v>
+      </c>
+      <c r="D33" t="s" s="15">
+        <v>78</v>
+      </c>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" t="s" s="15">
+        <v>137</v>
+      </c>
+      <c r="J33" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="K33" s="15"/>
+    </row>
+    <row r="34" ht="36" customHeight="1">
+      <c r="A34" s="24"/>
+      <c r="B34" s="31"/>
+      <c r="C34" t="s" s="29">
+        <v>38</v>
+      </c>
+      <c r="D34" t="s" s="15">
+        <v>80</v>
+      </c>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" t="s" s="15">
+        <v>138</v>
+      </c>
+      <c r="J34" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K34" s="15"/>
+    </row>
+    <row r="35" ht="14" customHeight="1">
+      <c r="A35" s="24"/>
+      <c r="B35" t="s" s="30">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s" s="29">
+        <v>39</v>
+      </c>
+      <c r="D35" t="s" s="15">
+        <v>78</v>
+      </c>
+      <c r="E35" s="16"/>
+      <c r="F35" t="s" s="15">
+        <v>78</v>
+      </c>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="K35" s="15"/>
+    </row>
+    <row r="36" ht="14" customHeight="1">
+      <c r="A36" s="24"/>
+      <c r="B36" t="s" s="30">
+        <v>6</v>
+      </c>
+      <c r="C36" s="34"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" t="s" s="15">
+        <v>98</v>
+      </c>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+    </row>
+    <row r="37" ht="245" customHeight="1">
+      <c r="A37" s="24"/>
+      <c r="B37" t="s" s="30">
+        <v>7</v>
+      </c>
+      <c r="C37" s="29"/>
+      <c r="D37" s="16"/>
+      <c r="E37" t="s" s="15">
+        <v>87</v>
+      </c>
+      <c r="F37" s="16"/>
+      <c r="G37" t="s" s="15">
+        <v>108</v>
+      </c>
+      <c r="H37" s="16"/>
+      <c r="I37" t="s" s="15">
+        <v>139</v>
+      </c>
+      <c r="J37" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="K37" s="15"/>
+    </row>
+    <row r="38" ht="47" customHeight="1">
+      <c r="A38" s="24"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="16"/>
+      <c r="E38" t="s" s="15">
+        <v>87</v>
+      </c>
+      <c r="F38" t="s" s="15">
+        <v>99</v>
+      </c>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="K38" s="15"/>
+    </row>
+    <row r="39" ht="47" customHeight="1">
+      <c r="A39" s="24"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="16"/>
+      <c r="E39" t="s" s="15">
+        <v>87</v>
+      </c>
+      <c r="F39" t="s" s="15">
+        <v>100</v>
+      </c>
+      <c r="G39" t="s" s="15">
+        <v>109</v>
+      </c>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="K39" s="15"/>
+    </row>
+    <row r="40" ht="47" customHeight="1">
+      <c r="A40" s="24"/>
+      <c r="B40" t="s" s="30">
+        <v>8</v>
+      </c>
+      <c r="C40" s="29"/>
+      <c r="D40" s="16"/>
+      <c r="E40" t="s" s="15">
+        <v>87</v>
+      </c>
+      <c r="F40" t="s" s="15">
+        <v>100</v>
+      </c>
+      <c r="G40" t="s" s="15">
+        <v>110</v>
+      </c>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" t="s" s="15">
+        <v>145</v>
+      </c>
+      <c r="K40" s="15"/>
+    </row>
+    <row r="41" ht="124" customHeight="1">
+      <c r="A41" s="24"/>
+      <c r="B41" t="s" s="30">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s" s="29">
+        <v>40</v>
+      </c>
+      <c r="D41" t="s" s="15">
+        <v>81</v>
+      </c>
+      <c r="E41" s="16"/>
+      <c r="F41" t="s" s="15">
+        <v>101</v>
+      </c>
+      <c r="G41" t="s" s="15">
+        <v>111</v>
+      </c>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="K41" s="15"/>
+    </row>
+    <row r="42" ht="102" customHeight="1">
+      <c r="A42" s="24"/>
+      <c r="B42" t="s" s="30">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s" s="29">
+        <v>41</v>
+      </c>
+      <c r="D42" t="s" s="15">
+        <v>81</v>
+      </c>
+      <c r="E42" s="16"/>
+      <c r="F42" t="s" s="15">
+        <v>102</v>
+      </c>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" t="s" s="15">
+        <v>140</v>
+      </c>
+      <c r="J42" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="K42" s="15"/>
+    </row>
+    <row r="43" ht="91" customHeight="1">
+      <c r="A43" s="24"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="16"/>
+      <c r="E43" t="s" s="15">
+        <v>87</v>
+      </c>
+      <c r="F43" t="s" s="15">
+        <v>103</v>
+      </c>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="K43" s="15"/>
+    </row>
+    <row r="44" ht="25" customHeight="1">
+      <c r="A44" s="24"/>
+      <c r="B44" t="s" s="30">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s" s="29">
+        <v>42</v>
+      </c>
+      <c r="D44" t="s" s="15">
+        <v>81</v>
+      </c>
+      <c r="E44" s="16"/>
+      <c r="F44" t="s" s="15">
+        <v>104</v>
+      </c>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K44" s="15"/>
+    </row>
+    <row r="45" ht="36" customHeight="1">
+      <c r="A45" s="24"/>
+      <c r="B45" s="36"/>
+      <c r="C45" t="s" s="29">
+        <v>43</v>
+      </c>
+      <c r="D45" t="s" s="15">
+        <v>82</v>
+      </c>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" t="s" s="15">
+        <v>144</v>
+      </c>
+      <c r="K45" s="15"/>
+    </row>
+    <row r="46" ht="58" customHeight="1">
+      <c r="A46" s="24"/>
+      <c r="B46" s="36"/>
+      <c r="C46" t="s" s="29">
+        <v>44</v>
+      </c>
+      <c r="D46" s="16"/>
+      <c r="E46" t="s" s="15">
+        <v>88</v>
+      </c>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" t="s" s="15">
+        <v>141</v>
+      </c>
+      <c r="J46" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K46" s="15"/>
+    </row>
+    <row r="47" ht="36" customHeight="1">
+      <c r="A47" s="24"/>
+      <c r="B47" s="36"/>
+      <c r="C47" t="s" s="29">
+        <v>45</v>
+      </c>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="K47" s="15"/>
+    </row>
+    <row r="48" ht="25" customHeight="1">
+      <c r="A48" s="24"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" t="s" s="15">
+        <v>112</v>
+      </c>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="K48" t="s" s="15">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" ht="14" customHeight="1">
+      <c r="A49" s="24"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" t="s" s="15">
+        <v>113</v>
+      </c>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="K49" t="s" s="15">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" ht="14" customHeight="1">
+      <c r="A50" s="24"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" t="s" s="15">
+        <v>114</v>
+      </c>
+      <c r="H50" s="16"/>
+      <c r="I50" s="16"/>
+      <c r="J50" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="K50" t="s" s="15">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" ht="14" customHeight="1">
+      <c r="A51" s="24"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" t="s" s="15">
+        <v>154</v>
+      </c>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+      <c r="J51" t="s" s="15">
+        <v>79</v>
+      </c>
+      <c r="K51" t="s" s="15">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" ht="58" customHeight="1">
+      <c r="A52" s="24"/>
+      <c r="B52" s="36"/>
+      <c r="C52" t="s" s="29">
+        <v>46</v>
+      </c>
+      <c r="D52" t="s" s="15">
+        <v>83</v>
+      </c>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+      <c r="J52" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K52" t="s" s="15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" ht="58" customHeight="1">
+      <c r="A53" s="24"/>
+      <c r="B53" s="36"/>
+      <c r="C53" t="s" s="29">
+        <v>47</v>
+      </c>
+      <c r="D53" t="s" s="15">
+        <v>84</v>
+      </c>
+      <c r="E53" t="s" s="15">
+        <v>89</v>
+      </c>
+      <c r="F53" s="16"/>
+      <c r="G53" t="s" s="15">
+        <v>116</v>
+      </c>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+      <c r="J53" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K53" t="s" s="15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" ht="36" customHeight="1">
+      <c r="A54" s="37"/>
+      <c r="B54" s="36"/>
+      <c r="C54" t="s" s="29">
+        <v>48</v>
+      </c>
+      <c r="D54" t="s" s="15">
+        <v>82</v>
+      </c>
+      <c r="E54" t="s" s="15">
+        <v>90</v>
+      </c>
+      <c r="F54" t="s" s="15">
+        <v>82</v>
+      </c>
+      <c r="G54" t="s" s="15">
+        <v>117</v>
+      </c>
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
+      <c r="J54" t="s" s="15">
+        <v>143</v>
+      </c>
+      <c r="K54" t="s" s="15">
+        <v>143</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:BC1"/>
-    <mergeCell ref="K2:W2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="X2:AE2"/>
-    <mergeCell ref="O3:S3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B11:B23"/>
+    <mergeCell ref="A1:A54"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AB3" r:id="rId1" location="" tooltip="" display=""/>
-    <hyperlink ref="AC3" r:id="rId2" location="" tooltip="" display=""/>
-    <hyperlink ref="C4" r:id="rId3" location="" tooltip="" display=""/>
-    <hyperlink ref="Z4" r:id="rId4" location="" tooltip="" display=""/>
-    <hyperlink ref="AA4" r:id="rId5" location="" tooltip="" display=""/>
-    <hyperlink ref="AB4" r:id="rId6" location="" tooltip="" display=""/>
-    <hyperlink ref="AC4" r:id="rId7" location="" tooltip="" display=""/>
-    <hyperlink ref="AD4" r:id="rId8" location="" tooltip="" display=""/>
-    <hyperlink ref="BA4" r:id="rId9" location="" tooltip="" display=""/>
-    <hyperlink ref="BA5" r:id="rId10" location="" tooltip="" display=""/>
-    <hyperlink ref="BA8" r:id="rId11" location="" tooltip="" display=""/>
+    <hyperlink ref="D15" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="D21" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="C28" r:id="rId3" location="" tooltip="" display=""/>
+    <hyperlink ref="C29" r:id="rId4" location="" tooltip="" display=""/>
+    <hyperlink ref="G53" r:id="rId5" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>